<commit_message>
merge changes with main
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -5,9 +5,41 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId3"/>
+    <sheet name="login" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+  <si>
+    <t>datakey</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>errormessage</t>
+  </si>
+  <si>
+    <t>Login_Valid</t>
+  </si>
+  <si>
+    <t>validuser</t>
+  </si>
+  <si>
+    <t>validpass</t>
+  </si>
+  <si>
+    <t>Login_InvalidUsername</t>
+  </si>
+  <si>
+    <t>invaliduser</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -23,6 +55,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -53,7 +90,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -78,16 +115,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -127,23 +179,35 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -166,7 +230,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -183,10 +247,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -363,11 +427,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -376,34 +443,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -651,12 +718,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -947,7 +1014,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1225,35 +1292,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5547" style="1" customWidth="1"/>
+    <col min="2" max="6" width="16.3516" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="A2" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>